<commit_message>
feat. new DataTable :Bottle -> TakeMedicineHistory / BottleMedicine, API Change, Test
</commit_message>
<xml_diff>
--- a/design/요구사항명세서.xlsx
+++ b/design/요구사항명세서.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parkkwonsoo/Desktop/Project/Capstone_Design_1/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281039B0-C4D3-C541-A3F3-306E0AC538CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2B297C-5CD4-7649-8FC3-CB1ECFE124B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="15940" activeTab="1" xr2:uid="{B5A5CC4F-DFB5-4B4E-83EE-885E37D02B5A}"/>
+    <workbookView xWindow="6940" yWindow="1540" windowWidth="28300" windowHeight="15940" activeTab="1" xr2:uid="{B5A5CC4F-DFB5-4B4E-83EE-885E37D02B5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Usage" sheetId="2" r:id="rId1"/>
     <sheet name="Data Table" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="128">
   <si>
     <t>Field</t>
   </si>
@@ -279,10 +280,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>약 등록 시 담당의 등록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>복용 잘 했는지 달력에 표시? -&gt; 성취도 향상</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -295,10 +292,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Bottle Open History</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>환자 특이사항 기록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -327,10 +320,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>피드백할 약병 : 관련 복용 약에 대한 피드백을 처방의가 전달함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>fdbType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -472,6 +461,86 @@
   </si>
   <si>
     <t>NUMBER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>feedback</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>약병에 약 등록 시 담당의 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담당의 관리 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담당의가 관리 요청 시 해당 기능 수락 및 보류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담당 환자 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환자를 등록할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 환자를 등록 요청 시, 환자가 수락하면 환자의 개인 정보 및 약병 관리 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BottleHistory 변경 시 수정해야 할 것들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Bottle API</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. MQTT API</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. Hub API</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. User API</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. Bottle History Schema</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. Bottle Schema</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. Doctor API</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BottleMedicineHistory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>takeMedicineHistory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bmId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피드백할 약에 대한 내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>regDtm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -546,7 +615,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -729,13 +798,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -841,6 +949,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -885,6 +1011,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1202,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014DD845-F766-E24A-A779-ADD3A5BFF279}">
   <dimension ref="B2:O33"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1213,79 +1342,82 @@
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="19" thickBot="1">
       <c r="B2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="2:15">
-      <c r="B3" s="44"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="35" t="s">
+      <c r="B3" s="50"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="35" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="35" t="s">
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="37"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="43"/>
     </row>
     <row r="4" spans="2:15">
-      <c r="B4" s="46"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="40"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="46"/>
     </row>
     <row r="5" spans="2:15" ht="19" thickBot="1">
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="43"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="49"/>
     </row>
     <row r="6" spans="2:15" ht="20" thickBot="1">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="37"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="25" t="s">
         <v>55</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="F6" s="26"/>
+        <v>89</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>110</v>
+      </c>
       <c r="G6" s="27"/>
       <c r="H6" s="25"/>
       <c r="I6" s="26"/>
@@ -1297,15 +1429,17 @@
       <c r="O6" s="27"/>
     </row>
     <row r="7" spans="2:15" ht="57">
-      <c r="B7" s="38"/>
-      <c r="C7" s="40"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="28" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="21"/>
+        <v>90</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>111</v>
+      </c>
       <c r="G7" s="29"/>
       <c r="H7" s="28"/>
       <c r="I7" s="21"/>
@@ -1317,10 +1451,10 @@
       <c r="O7" s="29"/>
     </row>
     <row r="8" spans="2:15" ht="38">
-      <c r="B8" s="38"/>
-      <c r="C8" s="40"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
@@ -1335,8 +1469,8 @@
       <c r="O8" s="29"/>
     </row>
     <row r="9" spans="2:15">
-      <c r="B9" s="38"/>
-      <c r="C9" s="40"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="28"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
@@ -1351,8 +1485,8 @@
       <c r="O9" s="29"/>
     </row>
     <row r="10" spans="2:15">
-      <c r="B10" s="38"/>
-      <c r="C10" s="40"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="28"/>
       <c r="E10" s="21"/>
       <c r="F10" s="21"/>
@@ -1367,8 +1501,8 @@
       <c r="O10" s="29"/>
     </row>
     <row r="11" spans="2:15">
-      <c r="B11" s="38"/>
-      <c r="C11" s="40"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="28"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
@@ -1383,8 +1517,8 @@
       <c r="O11" s="29"/>
     </row>
     <row r="12" spans="2:15" ht="19" thickBot="1">
-      <c r="B12" s="38"/>
-      <c r="C12" s="40"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="28"/>
       <c r="E12" s="21"/>
       <c r="F12" s="21"/>
@@ -1399,10 +1533,10 @@
       <c r="O12" s="29"/>
     </row>
     <row r="13" spans="2:15" ht="20" thickBot="1">
-      <c r="B13" s="38"/>
-      <c r="C13" s="40"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="26"/>
@@ -1417,10 +1551,10 @@
       <c r="O13" s="27"/>
     </row>
     <row r="14" spans="2:15" ht="38">
-      <c r="B14" s="38"/>
-      <c r="C14" s="40"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="46"/>
       <c r="D14" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
@@ -1435,8 +1569,8 @@
       <c r="O14" s="29"/>
     </row>
     <row r="15" spans="2:15">
-      <c r="B15" s="38"/>
-      <c r="C15" s="40"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="46"/>
       <c r="D15" s="28"/>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
@@ -1451,8 +1585,8 @@
       <c r="O15" s="29"/>
     </row>
     <row r="16" spans="2:15">
-      <c r="B16" s="38"/>
-      <c r="C16" s="40"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="28"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
@@ -1467,8 +1601,8 @@
       <c r="O16" s="29"/>
     </row>
     <row r="17" spans="2:15">
-      <c r="B17" s="38"/>
-      <c r="C17" s="40"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="46"/>
       <c r="D17" s="28"/>
       <c r="E17" s="21"/>
       <c r="F17" s="21"/>
@@ -1483,8 +1617,8 @@
       <c r="O17" s="29"/>
     </row>
     <row r="18" spans="2:15">
-      <c r="B18" s="38"/>
-      <c r="C18" s="40"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="28"/>
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
@@ -1499,8 +1633,8 @@
       <c r="O18" s="29"/>
     </row>
     <row r="19" spans="2:15" ht="19" thickBot="1">
-      <c r="B19" s="41"/>
-      <c r="C19" s="43"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="30"/>
       <c r="E19" s="31"/>
       <c r="F19" s="31"/>
@@ -1515,10 +1649,10 @@
       <c r="O19" s="32"/>
     </row>
     <row r="20" spans="2:15" ht="20" thickBot="1">
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="40"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="25"/>
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
@@ -1532,7 +1666,9 @@
       <c r="J20" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="27"/>
+      <c r="K20" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="L20" s="26" t="s">
         <v>59</v>
       </c>
@@ -1541,8 +1677,8 @@
       <c r="O20" s="27"/>
     </row>
     <row r="21" spans="2:15" ht="19">
-      <c r="B21" s="38"/>
-      <c r="C21" s="40"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="28"/>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
@@ -1552,9 +1688,11 @@
         <v>57</v>
       </c>
       <c r="J21" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="K21" s="29"/>
+        <v>88</v>
+      </c>
+      <c r="K21" s="29" t="s">
+        <v>113</v>
+      </c>
       <c r="L21" s="21" t="s">
         <v>58</v>
       </c>
@@ -1562,9 +1700,9 @@
       <c r="N21" s="21"/>
       <c r="O21" s="29"/>
     </row>
-    <row r="22" spans="2:15" ht="19">
-      <c r="B22" s="38"/>
-      <c r="C22" s="40"/>
+    <row r="22" spans="2:15" ht="76">
+      <c r="B22" s="44"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="28"/>
       <c r="E22" s="21"/>
       <c r="F22" s="21"/>
@@ -1574,9 +1712,11 @@
         <v>61</v>
       </c>
       <c r="J22" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="K22" s="29"/>
+        <v>87</v>
+      </c>
+      <c r="K22" s="29" t="s">
+        <v>114</v>
+      </c>
       <c r="L22" s="21" t="s">
         <v>60</v>
       </c>
@@ -1585,8 +1725,8 @@
       <c r="O22" s="29"/>
     </row>
     <row r="23" spans="2:15" ht="19">
-      <c r="B23" s="38"/>
-      <c r="C23" s="40"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="28"/>
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
@@ -1594,19 +1734,19 @@
       <c r="H23" s="28"/>
       <c r="I23" s="21"/>
       <c r="J23" s="34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K23" s="29"/>
       <c r="L23" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
       <c r="O23" s="29"/>
     </row>
     <row r="24" spans="2:15" ht="19">
-      <c r="B24" s="38"/>
-      <c r="C24" s="40"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="28"/>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
@@ -1616,15 +1756,15 @@
       <c r="J24" s="33"/>
       <c r="K24" s="29"/>
       <c r="L24" s="34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
       <c r="O24" s="29"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="B25" s="38"/>
-      <c r="C25" s="40"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="46"/>
       <c r="D25" s="28"/>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
@@ -1639,8 +1779,8 @@
       <c r="O25" s="29"/>
     </row>
     <row r="26" spans="2:15" ht="19" thickBot="1">
-      <c r="B26" s="38"/>
-      <c r="C26" s="40"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="46"/>
       <c r="D26" s="28"/>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
@@ -1655,8 +1795,8 @@
       <c r="O26" s="29"/>
     </row>
     <row r="27" spans="2:15" ht="19" thickBot="1">
-      <c r="B27" s="38"/>
-      <c r="C27" s="40"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="25"/>
       <c r="E27" s="26"/>
       <c r="F27" s="26"/>
@@ -1671,8 +1811,8 @@
       <c r="O27" s="27"/>
     </row>
     <row r="28" spans="2:15">
-      <c r="B28" s="38"/>
-      <c r="C28" s="40"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="46"/>
       <c r="D28" s="28"/>
       <c r="E28" s="21"/>
       <c r="F28" s="21"/>
@@ -1687,8 +1827,8 @@
       <c r="O28" s="29"/>
     </row>
     <row r="29" spans="2:15">
-      <c r="B29" s="38"/>
-      <c r="C29" s="40"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="46"/>
       <c r="D29" s="28"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
@@ -1703,8 +1843,8 @@
       <c r="O29" s="29"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="B30" s="38"/>
-      <c r="C30" s="40"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="46"/>
       <c r="D30" s="28"/>
       <c r="E30" s="21"/>
       <c r="F30" s="21"/>
@@ -1719,8 +1859,8 @@
       <c r="O30" s="29"/>
     </row>
     <row r="31" spans="2:15">
-      <c r="B31" s="38"/>
-      <c r="C31" s="40"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="46"/>
       <c r="D31" s="28"/>
       <c r="E31" s="21"/>
       <c r="F31" s="21"/>
@@ -1735,8 +1875,8 @@
       <c r="O31" s="29"/>
     </row>
     <row r="32" spans="2:15">
-      <c r="B32" s="38"/>
-      <c r="C32" s="40"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="46"/>
       <c r="D32" s="28"/>
       <c r="E32" s="21"/>
       <c r="F32" s="21"/>
@@ -1751,8 +1891,8 @@
       <c r="O32" s="29"/>
     </row>
     <row r="33" spans="2:15" ht="19" thickBot="1">
-      <c r="B33" s="41"/>
-      <c r="C33" s="43"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="49"/>
       <c r="D33" s="30"/>
       <c r="E33" s="31"/>
       <c r="F33" s="31"/>
@@ -1782,10 +1922,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E875DA9-9D29-664A-8FDC-92E4D61DDB36}">
-  <dimension ref="B3:U34"/>
+  <dimension ref="B3:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="87" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1803,7 +1943,7 @@
         <v>43</v>
       </c>
       <c r="Q3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="2:21" ht="19" thickBot="1">
@@ -1890,7 +2030,7 @@
         <v>12</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>22</v>
@@ -1933,7 +2073,7 @@
       </c>
       <c r="O6" s="16"/>
       <c r="Q6" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>14</v>
@@ -1993,13 +2133,13 @@
     </row>
     <row r="8" spans="2:21" ht="19" thickBot="1">
       <c r="B8" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E8" s="5" t="b">
         <v>0</v>
@@ -2018,19 +2158,19 @@
         <v>0</v>
       </c>
       <c r="O8" s="16"/>
-      <c r="Q8" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="R8" s="11" t="s">
+      <c r="Q8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U8" s="6"/>
-    </row>
-    <row r="9" spans="2:21">
+      <c r="S8" s="2"/>
+      <c r="T8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="U8" s="3"/>
+    </row>
+    <row r="9" spans="2:21" ht="19" thickBot="1">
       <c r="K9" s="15" t="s">
         <v>49</v>
       </c>
@@ -2044,10 +2184,23 @@
         <v>1</v>
       </c>
       <c r="O9" s="16"/>
+      <c r="Q9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="T9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="U9" s="6"/>
     </row>
     <row r="10" spans="2:21" ht="19" thickBot="1">
       <c r="B10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="K10" s="15" t="s">
         <v>47</v>
@@ -2062,9 +2215,6 @@
         <v>1</v>
       </c>
       <c r="O10" s="16"/>
-      <c r="Q10" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="11" spans="2:21" ht="19" thickBot="1">
       <c r="B11" s="12" t="s">
@@ -2095,23 +2245,11 @@
         <v>1</v>
       </c>
       <c r="O11" s="19"/>
-      <c r="Q11" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="R11" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="S11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="T11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="U11" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21">
+      <c r="Q11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" ht="19" thickBot="1">
       <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
@@ -2123,25 +2261,27 @@
         <v>0</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="U12" s="3" t="s">
-        <v>12</v>
+        <v>104</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="T12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="U12" s="10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:21" ht="19" thickBot="1">
       <c r="B13" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>14</v>
@@ -2152,28 +2292,28 @@
       </c>
       <c r="F13" s="16"/>
       <c r="K13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:21" ht="19" thickBot="1">
       <c r="B14" s="15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20" t="b">
@@ -2196,7 +2336,7 @@
         <v>9</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="R14" s="2" t="s">
         <v>14</v>
@@ -2205,11 +2345,13 @@
       <c r="T14" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="U14" s="3"/>
+      <c r="U14" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="2:21">
       <c r="B15" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>14</v>
@@ -2219,30 +2361,28 @@
         <v>0</v>
       </c>
       <c r="F15" s="16"/>
-      <c r="K15" s="1" t="s">
+      <c r="K15" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O15" s="3" t="s">
+      <c r="M15" s="36"/>
+      <c r="N15" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" s="37" t="s">
         <v>12</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="R15" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="R15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S15" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="T15" s="7" t="b">
-        <v>1</v>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="U15" s="3"/>
     </row>
@@ -2253,7 +2393,7 @@
       <c r="E16" s="18"/>
       <c r="F16" s="19"/>
       <c r="K16" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>31</v>
@@ -2265,14 +2405,17 @@
         <v>0</v>
       </c>
       <c r="O16" s="3"/>
+      <c r="P16" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="Q16" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="R16" s="7" t="s">
         <v>14</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T16" s="7" t="b">
         <v>1</v>
@@ -2281,27 +2424,30 @@
     </row>
     <row r="17" spans="2:21">
       <c r="K17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>22</v>
+        <v>72</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="O17" s="3" t="s">
-        <v>18</v>
+      <c r="O17" s="3"/>
+      <c r="P17" t="s">
+        <v>75</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="R17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2" t="b">
-        <v>0</v>
+      <c r="S17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="T17" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="U17" s="3"/>
     </row>
@@ -2309,32 +2455,33 @@
       <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="K18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L18" s="11" t="s">
+      <c r="K18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O18" s="6" t="s">
+      <c r="M18" s="2"/>
+      <c r="N18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q18" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="R18" s="11" t="s">
+      <c r="P18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S18" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="T18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U18" s="6"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U18" s="3"/>
     </row>
     <row r="19" spans="2:21" ht="19" thickBot="1">
       <c r="B19" s="8" t="s">
@@ -2352,6 +2499,35 @@
       <c r="F19" s="10" t="s">
         <v>9</v>
       </c>
+      <c r="K19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P19" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="R19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="S19" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="T19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="U19" s="6"/>
     </row>
     <row r="20" spans="2:21" ht="19" thickBot="1">
       <c r="B20" s="1" t="s">
@@ -2367,8 +2543,18 @@
       <c r="F20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K20" t="s">
-        <v>70</v>
+      <c r="K20" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:21" ht="19" thickBot="1">
@@ -2385,21 +2571,6 @@
         <v>1</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="K21" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L21" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="M21" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="N21" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="O21" s="10" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="22" spans="2:21" ht="19" thickBot="1">
       <c r="B22" s="4" t="s">
@@ -2417,270 +2588,417 @@
       <c r="F22" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L22" s="2" t="s">
+      <c r="K22" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="L22" s="23"/>
+    </row>
+    <row r="23" spans="2:21" ht="19">
+      <c r="K23" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" ht="19" thickBot="1">
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" ht="19" thickBot="1">
+      <c r="B25" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" ht="19" thickBot="1">
+      <c r="B26" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O22" s="3" t="s">
+      <c r="D26" s="20"/>
+      <c r="E26" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" ht="19" thickBot="1">
+      <c r="B27" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" ht="19" thickBot="1">
+      <c r="B30" t="s">
+        <v>124</v>
+      </c>
+      <c r="K30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21">
+      <c r="B31" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="K31" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="L31" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="M31" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="N31" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="O31" s="40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21">
+      <c r="B32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="2:21">
-      <c r="K23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L23" s="2" t="s">
+      <c r="K32" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17">
+      <c r="B33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M23" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N23" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O23" s="3"/>
-      <c r="P23" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="2:21">
-      <c r="K24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L24" s="2" t="s">
+      <c r="E33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="K33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17">
+      <c r="B34" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L34" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O34" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17">
+      <c r="B35" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="20">
+        <v>0</v>
+      </c>
+      <c r="E35" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" s="16"/>
+      <c r="K35" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L35" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O24" s="3"/>
-      <c r="P24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="2:21" ht="19" thickBot="1">
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L25" s="7" t="s">
+      <c r="M35" s="20"/>
+      <c r="N35" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O35" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17">
+      <c r="B36" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="20">
+        <v>0</v>
+      </c>
+      <c r="E36" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" s="16"/>
+      <c r="K36" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="L36" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="M36" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="N36" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O36" s="16"/>
+      <c r="Q36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" ht="19" thickBot="1">
+      <c r="B37" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P25" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="2:21" ht="19" thickBot="1">
-      <c r="B26" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L26" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O26" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="P26" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="2:21" ht="19" thickBot="1">
-      <c r="B27" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="20" t="s">
+      <c r="D37" s="18">
+        <v>0</v>
+      </c>
+      <c r="E37" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="19"/>
+      <c r="G37" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" t="s">
+        <v>41</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="L37" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="2:21">
-      <c r="B28" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="20">
-        <v>0</v>
-      </c>
-      <c r="E28" s="20" t="b">
+      <c r="M37" s="18">
+        <v>0</v>
+      </c>
+      <c r="N37" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="F28" s="16"/>
-      <c r="K28" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="L28" s="23"/>
-    </row>
-    <row r="29" spans="2:21" ht="19">
-      <c r="B29" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="20">
-        <v>0</v>
-      </c>
-      <c r="E29" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" s="16"/>
-      <c r="K29" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="2:21">
-      <c r="B30" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="20">
-        <v>0</v>
-      </c>
-      <c r="E30" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" s="16"/>
-      <c r="K30" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="2:21">
-      <c r="B31" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="2:21" ht="19" thickBot="1">
-      <c r="B32" s="15" t="s">
+      <c r="O37" s="19"/>
+      <c r="P37" t="s">
         <v>34</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="20">
-        <v>0</v>
-      </c>
-      <c r="E32" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" s="16"/>
-      <c r="G32" t="s">
-        <v>30</v>
-      </c>
-      <c r="H32" t="s">
-        <v>41</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L32" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8">
-      <c r="B33" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="19" thickBot="1">
-      <c r="B34" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" t="s">
-        <v>34</v>
-      </c>
-      <c r="H34" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C575262B-E2B7-8A47-8185-84B6719C8DDF}">
+  <dimension ref="B2:D1048576"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="B2" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="56" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+    </row>
+    <row r="1048576" spans="2:4">
+      <c r="B1048576" s="56"/>
+      <c r="C1048576" s="56"/>
+      <c r="D1048576" s="56"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B1048576:D1048576"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat. get all bottle List api implement
</commit_message>
<xml_diff>
--- a/design/요구사항명세서.xlsx
+++ b/design/요구사항명세서.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parkkwonsoo/Desktop/Project/Capstone_Design_1/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2B297C-5CD4-7649-8FC3-CB1ECFE124B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D2B870-FC10-2F49-8BF1-B091E94D5F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6940" yWindow="1540" windowWidth="28300" windowHeight="15940" activeTab="1" xr2:uid="{B5A5CC4F-DFB5-4B4E-83EE-885E37D02B5A}"/>
+    <workbookView xWindow="5620" yWindow="500" windowWidth="32780" windowHeight="19120" activeTab="2" xr2:uid="{B5A5CC4F-DFB5-4B4E-83EE-885E37D02B5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Usage" sheetId="2" r:id="rId1"/>
     <sheet name="Data Table" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="어플리케이션 시나리오" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="195">
   <si>
     <t>Field</t>
   </si>
@@ -492,38 +492,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BottleHistory 변경 시 수정해야 할 것들</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Bottle API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. MQTT API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. Hub API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4. User API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5. Bottle History Schema</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6. Bottle Schema</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7. Doctor API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BottleMedicineHistory</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -541,6 +509,324 @@
   </si>
   <si>
     <t>regDtm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>약병관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>약 및 담당의 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피드백 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>약병 해제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나의 메뉴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대분류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소분류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>API</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Next Action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허브관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>약병 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허브 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허브 해제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담당의 등록 요청 리스트 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>약병 정보 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입을 한다 : 입력 값
+{ userId, password, passwordCheck, userNm, userAge, contact }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST : http://localhost:4000/api/auth/register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성공 시 로그인 페이지로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성공 시 메인화면으로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST : http://localhost:4000/api/auth/login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인을 한다 : 입력 값
+{ userId, password }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그아웃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허브관리 / 약병관리 / 나의 메뉴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메뉴 선택 후 해당 컴포넌트로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다른 메뉴로 접근 가능 한 메인 화면. 초기 화면은 약병 리스트 띄우는 것. 탭 네비게이션바, 버거 메뉴 등. 구현 가능한 범위에서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새로운 허브를 등록한다 : 입력 값
+{ hubId, host, port }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST : http://localhost:4000/api/hub</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허브 등록 성공 시, 약병 등록 메뉴로 이동. 건너뛰기 시 메인 메뉴로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허브 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허브를 해제한다 : 입력 값
+null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE : http://localhost:4000/api/hub/${hubId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허브 해제 성공 시 허브 리스트 메뉴로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저에 등록된 허브 리스트를 출력한다 : 입력 값 null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET : http://localhost:4000/api/hub</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허브 리스트에서 특정 허브 클릭 시, 해당 허브에 연결된 약병 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>특정 허브 연결된 약병 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 약병 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET : http://localhost:4000/api/bottle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET : http://localhost:4000/api/bottle/hub/${hubId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE : http://localhost:4000/api/bottle/${bottleId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET : http://localhost:4000/api/bottle/${bottleId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET : http://localhost:4000/api/bottle/feedback/${bottleId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PATCH : http://localhost:4000/api/bottle/${bottleId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST : http://localhost:4000/api/bottle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내 정보 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새로운 약병을 등록한다. 입력 값
+{ bottleId, hubId }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>약병 등록 성공 후, 약 및 담당의 등록 컴포넌트로 이동
+건너뛰기 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>약병에 약, 복용량, 처방의를 등록한다. : 입력 값
+{ medicineId, dosage, doctorId }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>약 검색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>키워드로 약 검색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>처방의는 생략 가능, 약 및 담당의를 등록하면 메인 컴포넌트로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>처방의가 남긴 약 복용에 관한 피드백 내역을 확인한다. 해당 내역은 현재 약병에 등록된 약에 관한 피드백만을 확인한다.
+입력 값 : null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>약병에 관한 상세 정보를 조회한다. 해당 약병에 대한 복용 내역을 확인 가능하다. 리스트 형태로 리턴됨
+입력 값 : null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 약병을 해제한다. 해당 약병에 관한 정보들을 모두 지운다.
+입력 값 : null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>약병 해제 성공 시, 약병 리스트로 돌아감.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신의 허브에 등록된 약병을 조회한다. 자신의 허브가 아닐 경우 error
+입력 값 : null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신에게 등록된 모든 약병을 보여준다. 허브 상관 없이 보여줌
+입력 값 : null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET : http://localhost:4000/api/user/doctorrequest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담당의가 요청한 내역을 보여준다. 
+입력 값 : null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST : http://localhost:4000/api/user/doctorrequest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수락 시 이전 페이지(= 마이 페이지)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내 정보를 가져온다
+입력 값 : null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담당의 등록 요청을 수락한다.
+입력 값 : { doctorId }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> GET : http://localhost:4000/api/user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그아웃 한다.
+입력 값 : null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>특정 약 상세 정보 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST : http://localhost:4000/api/auth/logout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>키워드로 약을 검색함. 해당 키워드 하나로 약 명, 제조사명, 약효 모두 검색 가능
+입력 값 :  { keyword }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST : http://localhost:4000/api/medicine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>특정 약의 정보를 조회함
+입력 값 : null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET : http://localhost:4000/api/medicine/${medicineId}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -548,7 +834,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -588,8 +874,17 @@
       <family val="2"/>
       <charset val="129"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,6 +909,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -843,7 +1144,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1012,8 +1313,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1924,7 +2258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E875DA9-9D29-664A-8FDC-92E4D61DDB36}">
   <dimension ref="B3:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="87" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="87" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -2456,7 +2790,7 @@
         <v>20</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="L18" s="7" t="s">
         <v>22</v>
@@ -2469,7 +2803,7 @@
         <v>18</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>98</v>
@@ -2673,10 +3007,10 @@
     </row>
     <row r="30" spans="2:21" ht="19" thickBot="1">
       <c r="B30" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="K30" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="2:21">
@@ -2726,7 +3060,7 @@
         <v>12</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>22</v>
@@ -2769,7 +3103,7 @@
     </row>
     <row r="34" spans="2:17">
       <c r="B34" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>22</v>
@@ -2838,7 +3172,7 @@
       </c>
       <c r="F36" s="16"/>
       <c r="K36" s="15" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L36" s="20" t="s">
         <v>31</v>
@@ -2898,105 +3232,926 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C575262B-E2B7-8A47-8185-84B6719C8DDF}">
-  <dimension ref="B2:D1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5205B6E-3925-2641-B69B-FE329201EAC4}">
+  <dimension ref="B1:P39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="4" max="5" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:4">
-      <c r="B2" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="56"/>
+    <row r="1" spans="2:16" ht="19" thickBot="1">
+      <c r="B1" s="66" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64" t="s">
+        <v>130</v>
+      </c>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64" t="s">
+        <v>131</v>
+      </c>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="67"/>
+    </row>
+    <row r="2" spans="2:16">
+      <c r="B2" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="58"/>
       <c r="D2" s="56"/>
-    </row>
-    <row r="3" spans="2:4">
-      <c r="B3" s="56" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="53"/>
+    </row>
+    <row r="3" spans="2:16" ht="42" customHeight="1">
+      <c r="B3" s="59"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="56"/>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="56" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="53"/>
+    </row>
+    <row r="4" spans="2:16">
+      <c r="B4" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="58"/>
       <c r="D4" s="56"/>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="56" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="53"/>
+    </row>
+    <row r="5" spans="2:16">
+      <c r="B5" s="59"/>
+      <c r="C5" s="58"/>
       <c r="D5" s="56"/>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="56" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="56" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="53"/>
+    </row>
+    <row r="6" spans="2:16">
+      <c r="B6" s="59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="58"/>
+      <c r="D6" s="56" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="56" t="s">
+        <v>146</v>
+      </c>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="53"/>
+    </row>
+    <row r="7" spans="2:16" ht="56" customHeight="1">
+      <c r="B7" s="59"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="56"/>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="56" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="56" t="s">
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="53"/>
+    </row>
+    <row r="8" spans="2:16">
+      <c r="B8" s="59" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="58"/>
+      <c r="D8" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="58" t="s">
+        <v>149</v>
+      </c>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="N8" s="56"/>
+      <c r="O8" s="56"/>
+      <c r="P8" s="53"/>
+    </row>
+    <row r="9" spans="2:16" ht="36" customHeight="1">
+      <c r="B9" s="59"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="53"/>
+    </row>
+    <row r="10" spans="2:16">
+      <c r="B10" s="59"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="56" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="N10" s="56"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="53"/>
+    </row>
+    <row r="11" spans="2:16">
+      <c r="B11" s="59"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="53"/>
+    </row>
+    <row r="12" spans="2:16">
+      <c r="B12" s="59"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56" t="s">
+        <v>155</v>
+      </c>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="58" t="s">
+        <v>156</v>
+      </c>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="56" t="s">
+        <v>157</v>
+      </c>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="53"/>
+    </row>
+    <row r="13" spans="2:16" ht="39" customHeight="1">
+      <c r="B13" s="59"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="56"/>
+      <c r="P13" s="53"/>
+    </row>
+    <row r="14" spans="2:16">
+      <c r="B14" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-    </row>
-    <row r="1048576" spans="2:4">
-      <c r="B1048576" s="56"/>
-      <c r="C1048576" s="56"/>
-      <c r="D1048576" s="56"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="N14" s="56"/>
+      <c r="O14" s="56"/>
+      <c r="P14" s="53"/>
+    </row>
+    <row r="15" spans="2:16" ht="58" customHeight="1">
+      <c r="B15" s="59"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="56"/>
+      <c r="P15" s="53"/>
+    </row>
+    <row r="16" spans="2:16">
+      <c r="B16" s="59"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="56" t="s">
+        <v>173</v>
+      </c>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="53"/>
+    </row>
+    <row r="17" spans="2:16" ht="40" customHeight="1">
+      <c r="B17" s="59"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="53"/>
+    </row>
+    <row r="18" spans="2:16">
+      <c r="B18" s="59"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56" t="s">
+        <v>174</v>
+      </c>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="56"/>
+      <c r="P18" s="53"/>
+    </row>
+    <row r="19" spans="2:16" ht="70" customHeight="1">
+      <c r="B19" s="59"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="56"/>
+      <c r="O19" s="56"/>
+      <c r="P19" s="53"/>
+    </row>
+    <row r="20" spans="2:16">
+      <c r="B20" s="59"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="58" t="s">
+        <v>163</v>
+      </c>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="56"/>
+      <c r="P20" s="53"/>
+    </row>
+    <row r="21" spans="2:16" ht="78" customHeight="1">
+      <c r="B21" s="59"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="56"/>
+      <c r="P21" s="53"/>
+    </row>
+    <row r="22" spans="2:16">
+      <c r="B22" s="59"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="58" t="s">
+        <v>162</v>
+      </c>
+      <c r="J22" s="58"/>
+      <c r="K22" s="58"/>
+      <c r="L22" s="58"/>
+      <c r="M22" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="N22" s="56"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="53"/>
+    </row>
+    <row r="23" spans="2:16" ht="50" customHeight="1">
+      <c r="B23" s="59"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="56"/>
+      <c r="P23" s="53"/>
+    </row>
+    <row r="24" spans="2:16">
+      <c r="B24" s="59"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="56" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="58" t="s">
+        <v>161</v>
+      </c>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
+      <c r="O24" s="56"/>
+      <c r="P24" s="53"/>
+    </row>
+    <row r="25" spans="2:16" ht="49" customHeight="1">
+      <c r="B25" s="59"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="56"/>
+      <c r="P25" s="53"/>
+    </row>
+    <row r="26" spans="2:16">
+      <c r="B26" s="59"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56" t="s">
+        <v>179</v>
+      </c>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="J26" s="58"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="60"/>
+      <c r="N26" s="60"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="61"/>
+    </row>
+    <row r="27" spans="2:16" ht="46" customHeight="1">
+      <c r="B27" s="59"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="58"/>
+      <c r="J27" s="58"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="60"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="61"/>
+    </row>
+    <row r="28" spans="2:16">
+      <c r="B28" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="58"/>
+      <c r="D28" s="56" t="s">
+        <v>136</v>
+      </c>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="J28" s="58"/>
+      <c r="K28" s="58"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="60"/>
+      <c r="P28" s="61"/>
+    </row>
+    <row r="29" spans="2:16" ht="35" customHeight="1">
+      <c r="B29" s="59"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="60"/>
+      <c r="N29" s="60"/>
+      <c r="O29" s="60"/>
+      <c r="P29" s="61"/>
+    </row>
+    <row r="30" spans="2:16">
+      <c r="B30" s="59"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="58" t="s">
+        <v>182</v>
+      </c>
+      <c r="J30" s="58"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="N30" s="56"/>
+      <c r="O30" s="56"/>
+      <c r="P30" s="53"/>
+    </row>
+    <row r="31" spans="2:16">
+      <c r="B31" s="59"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="53"/>
+    </row>
+    <row r="32" spans="2:16">
+      <c r="B32" s="59"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56" t="s">
+        <v>184</v>
+      </c>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="58" t="s">
+        <v>186</v>
+      </c>
+      <c r="J32" s="58"/>
+      <c r="K32" s="58"/>
+      <c r="L32" s="58"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="53"/>
+    </row>
+    <row r="33" spans="2:16">
+      <c r="B33" s="59"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="58"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="58"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="56"/>
+      <c r="O33" s="56"/>
+      <c r="P33" s="53"/>
+    </row>
+    <row r="34" spans="2:16">
+      <c r="B34" s="59"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="56" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56" t="s">
+        <v>187</v>
+      </c>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="J34" s="58"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="58"/>
+      <c r="M34" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="N34" s="56"/>
+      <c r="O34" s="56"/>
+      <c r="P34" s="53"/>
+    </row>
+    <row r="35" spans="2:16">
+      <c r="B35" s="59"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="58"/>
+      <c r="J35" s="58"/>
+      <c r="K35" s="58"/>
+      <c r="L35" s="58"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="56"/>
+      <c r="O35" s="56"/>
+      <c r="P35" s="53"/>
+    </row>
+    <row r="36" spans="2:16">
+      <c r="B36" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="C36" s="58"/>
+      <c r="D36" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56" t="s">
+        <v>191</v>
+      </c>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="J36" s="58"/>
+      <c r="K36" s="58"/>
+      <c r="L36" s="58"/>
+      <c r="M36" s="56"/>
+      <c r="N36" s="56"/>
+      <c r="O36" s="56"/>
+      <c r="P36" s="53"/>
+    </row>
+    <row r="37" spans="2:16" ht="55" customHeight="1">
+      <c r="B37" s="59"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="58"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="58"/>
+      <c r="L37" s="58"/>
+      <c r="M37" s="56"/>
+      <c r="N37" s="56"/>
+      <c r="O37" s="56"/>
+      <c r="P37" s="53"/>
+    </row>
+    <row r="38" spans="2:16">
+      <c r="B38" s="59"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="56" t="s">
+        <v>188</v>
+      </c>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56" t="s">
+        <v>193</v>
+      </c>
+      <c r="G38" s="56"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="J38" s="58"/>
+      <c r="K38" s="58"/>
+      <c r="L38" s="58"/>
+      <c r="M38" s="56"/>
+      <c r="N38" s="56"/>
+      <c r="O38" s="56"/>
+      <c r="P38" s="53"/>
+    </row>
+    <row r="39" spans="2:16" ht="36" customHeight="1" thickBot="1">
+      <c r="B39" s="62"/>
+      <c r="C39" s="63"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="57"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="63"/>
+      <c r="K39" s="63"/>
+      <c r="L39" s="63"/>
+      <c r="M39" s="57"/>
+      <c r="N39" s="57"/>
+      <c r="O39" s="57"/>
+      <c r="P39" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B1048576:D1048576"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
+  <mergeCells count="88">
+    <mergeCell ref="M36:P37"/>
+    <mergeCell ref="D38:E39"/>
+    <mergeCell ref="F38:H39"/>
+    <mergeCell ref="I38:L39"/>
+    <mergeCell ref="M38:P39"/>
+    <mergeCell ref="B36:C39"/>
+    <mergeCell ref="M32:P33"/>
+    <mergeCell ref="D34:E35"/>
+    <mergeCell ref="B28:C35"/>
+    <mergeCell ref="F34:H35"/>
+    <mergeCell ref="I34:L35"/>
+    <mergeCell ref="M34:P35"/>
+    <mergeCell ref="D36:E37"/>
+    <mergeCell ref="F36:H37"/>
+    <mergeCell ref="I36:L37"/>
+    <mergeCell ref="D28:E29"/>
+    <mergeCell ref="D30:E31"/>
+    <mergeCell ref="D32:E33"/>
+    <mergeCell ref="B14:C27"/>
+    <mergeCell ref="F32:H33"/>
+    <mergeCell ref="I32:L33"/>
+    <mergeCell ref="D8:E9"/>
+    <mergeCell ref="D10:E11"/>
+    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="D4:E5"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="D12:E13"/>
+    <mergeCell ref="B8:C13"/>
+    <mergeCell ref="M24:P25"/>
+    <mergeCell ref="M26:P27"/>
+    <mergeCell ref="M28:P29"/>
+    <mergeCell ref="M30:P31"/>
+    <mergeCell ref="D14:E15"/>
+    <mergeCell ref="D24:E25"/>
+    <mergeCell ref="D26:E27"/>
+    <mergeCell ref="M12:P13"/>
+    <mergeCell ref="M14:P15"/>
+    <mergeCell ref="M16:P17"/>
+    <mergeCell ref="M18:P19"/>
+    <mergeCell ref="M20:P21"/>
+    <mergeCell ref="M22:P23"/>
+    <mergeCell ref="I24:L25"/>
+    <mergeCell ref="I26:L27"/>
+    <mergeCell ref="I28:L29"/>
+    <mergeCell ref="I30:L31"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="M2:P3"/>
+    <mergeCell ref="M4:P5"/>
+    <mergeCell ref="M6:P7"/>
+    <mergeCell ref="M8:P9"/>
+    <mergeCell ref="M10:P11"/>
+    <mergeCell ref="I12:L13"/>
+    <mergeCell ref="I14:L15"/>
+    <mergeCell ref="I16:L17"/>
+    <mergeCell ref="I18:L19"/>
+    <mergeCell ref="I20:L21"/>
+    <mergeCell ref="I22:L23"/>
+    <mergeCell ref="F26:H27"/>
+    <mergeCell ref="F28:H29"/>
+    <mergeCell ref="F30:H31"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="I2:L3"/>
+    <mergeCell ref="I4:L5"/>
+    <mergeCell ref="I6:L7"/>
+    <mergeCell ref="I8:L9"/>
+    <mergeCell ref="I10:L11"/>
+    <mergeCell ref="F12:H13"/>
+    <mergeCell ref="F14:H15"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="F18:H19"/>
+    <mergeCell ref="F20:H21"/>
+    <mergeCell ref="F22:H23"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F2:H3"/>
+    <mergeCell ref="F4:H5"/>
+    <mergeCell ref="F6:H7"/>
+    <mergeCell ref="F8:H9"/>
+    <mergeCell ref="F10:H11"/>
+    <mergeCell ref="F24:H25"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="D18:E19"/>
+    <mergeCell ref="D20:E21"/>
+    <mergeCell ref="D22:E23"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>